<commit_message>
lot of work here
</commit_message>
<xml_diff>
--- a/Lucky.xlsx
+++ b/Lucky.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ysuprod-my.sharepoint.com/personal/gkerns_ysu_edu/Documents/Teaching/3473/23X/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkerns\Git\gh\luckyCharms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{A3A8D341-B2DA-48D0-9391-46D1EF92D89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADC0BC0A-36E8-4ED9-8E7B-F0F5807F2E8F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08E2FC6-909A-4330-A918-227739F515D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="750" windowWidth="18675" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="19800" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,21 +405,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B70"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="16.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -463,7 +463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -509,7 +509,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -555,7 +555,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -601,7 +601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -647,7 +647,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -693,7 +693,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -739,7 +739,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -785,7 +785,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -831,7 +831,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -877,7 +877,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -923,7 +923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -969,7 +969,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>4</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>4</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>5</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>5</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>5</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>5</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>5</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>5</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>5</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>5</v>
       </c>
@@ -3085,12 +3085,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>5</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C59">
         <v>58</v>
@@ -3131,7 +3131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>6</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>6</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>6</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>6</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>6</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>6</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>6</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>6</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>6</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>6</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>6</v>
       </c>
@@ -3644,6 +3644,68 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Math_Settings xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Owner xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Is_Collaboration_Space_Locked xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <FolderType xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <AppVersion xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Has_Leaders_Only_SectionGroup xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <TeamsChannelId xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Invited_Leaders xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Invited_Members xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <_activity xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Templates xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Members xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Self_Registration_Enabled xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <CultureName xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Distribution_Groups xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Member_Groups xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <NotebookType xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <Leaders xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <LMS_Mappings xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA61BEA16AD6D945B8DA45BB2ADD7DE2" ma:contentTypeVersion="36" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0867b9dc880043a13c923c6c7fd485f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="46fa9c9f-fda4-491b-85b4-963ba3579ba1" xmlns:ns4="78f2cd39-2627-4bc0-b74c-cc8d7db39831" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b888f60b95cd8ed01f3d930f9e541a2c" ns3:_="" ns4:_="">
     <xsd:import namespace="46fa9c9f-fda4-491b-85b4-963ba3579ba1"/>
@@ -4072,83 +4134,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Math_Settings xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Owner xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Is_Collaboration_Space_Locked xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <FolderType xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <AppVersion xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Has_Leaders_Only_SectionGroup xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <TeamsChannelId xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Invited_Leaders xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Invited_Members xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <_activity xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Templates xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Members xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Self_Registration_Enabled xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <CultureName xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Distribution_Groups xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Member_Groups xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <NotebookType xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <Leaders xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <LMS_Mappings xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="78f2cd39-2627-4bc0-b74c-cc8d7db39831" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF80DBB7-3B68-4511-9BDD-E801C4B8E4FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D23BBD-9200-4A1C-ABE6-A16002B1FDB5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="46fa9c9f-fda4-491b-85b4-963ba3579ba1"/>
-    <ds:schemaRef ds:uri="78f2cd39-2627-4bc0-b74c-cc8d7db39831"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4171,9 +4160,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D23BBD-9200-4A1C-ABE6-A16002B1FDB5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF80DBB7-3B68-4511-9BDD-E801C4B8E4FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="46fa9c9f-fda4-491b-85b4-963ba3579ba1"/>
+    <ds:schemaRef ds:uri="78f2cd39-2627-4bc0-b74c-cc8d7db39831"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>